<commit_message>
config & test case updated
</commit_message>
<xml_diff>
--- a/TestData/DriverHighLevelRegression.xlsx
+++ b/TestData/DriverHighLevelRegression.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Automation Tests" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Automation Tests'!$A$1:$F$60</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="202">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Invitation sent successfully</t>
   </si>
   <si>
-    <t>Invitation cancelled successfully</t>
-  </si>
-  <si>
     <t>Invitation accepted successfully</t>
   </si>
   <si>
@@ -65,17 +62,6 @@
   </si>
   <si>
     <t>User deleted successfully</t>
-  </si>
-  <si>
-    <t>To validate invite via email based on following conditions
-1) Launch application and login as global admin.
-2) Click on Users Menu.
-3) Click on Add User button.
-4) Enter valid details in required field (Full Name, Email)
-5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
-6) Select any one value from Carrier Drop Down field
-7) Click on Invite button and check invitation email sent successfully.
-8.) Clickon cancel invitation and check if invitation cancelled.</t>
   </si>
   <si>
     <t>To validate invite via email for Shipper Admin  based on following conditions
@@ -1098,9 +1084,6 @@
 </t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>User_TC010</t>
   </si>
   <si>
@@ -1158,7 +1141,7 @@
     <t>CancelShippers_TC004</t>
   </si>
   <si>
-    <t>group_Chat_TC004</t>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1550,9 +1533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1588,10 +1573,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1599,15 +1584,15 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -1615,50 +1600,50 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="181.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1671,7 +1656,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -1687,7 +1672,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -1703,7 +1688,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -1711,143 +1696,143 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>191</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="165.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="C12" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="165.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>202</v>
+        <v>18</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>20</v>
+        <v>201</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D16" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>33</v>
@@ -1857,192 +1842,192 @@
     </row>
     <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>201</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>200</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>195</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>203</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>198</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>199</v>
+        <v>60</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="375" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2052,205 +2037,205 @@
         <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="375" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" ht="375" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="375" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -2260,61 +2245,61 @@
         <v>101</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>109</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2327,26 +2312,26 @@
         <v>114</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -2359,15 +2344,15 @@
         <v>132</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>133</v>
       </c>
@@ -2375,42 +2360,42 @@
         <v>134</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -2423,10 +2408,10 @@
         <v>121</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -2439,26 +2424,26 @@
         <v>123</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -2471,26 +2456,26 @@
         <v>128</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
     </row>
-    <row r="58" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -2503,10 +2488,10 @@
         <v>138</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -2519,95 +2504,95 @@
         <v>140</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D65" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
     </row>
-    <row r="66" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>151</v>
       </c>
@@ -2615,15 +2600,15 @@
         <v>152</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
     </row>
-    <row r="67" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>153</v>
       </c>
@@ -2631,31 +2616,31 @@
         <v>154</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>158</v>
       </c>
@@ -2663,26 +2648,26 @@
         <v>159</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -2695,61 +2680,59 @@
         <v>164</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>165</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="C73" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="B74" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="C74" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
+        <v>160</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -2759,10 +2742,10 @@
         <v>172</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="210" x14ac:dyDescent="0.25">
@@ -2773,13 +2756,13 @@
         <v>174</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>175</v>
       </c>
@@ -2787,55 +2770,55 @@
         <v>176</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>186</v>
       </c>
@@ -2843,10 +2826,10 @@
         <v>187</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -2857,28 +2840,14 @@
         <v>189</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F61"/>
+  <autoFilter ref="A1:F60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
scripts config and Test Data updated
</commit_message>
<xml_diff>
--- a/TestData/DriverHighLevelRegression.xlsx
+++ b/TestData/DriverHighLevelRegression.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="208">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -1174,9 +1174,6 @@
 5) Select any one role (Carrier, Shipper Admin, Shipper User, Driver (Full) and Driver (Limited) .
 6) Select any one value from Carrier Drop Down field.
 7) Click on cancel Invite button and check cancelled successfully.</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1570,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C84"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,7 +1784,7 @@
         <v>197</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>198</v>
@@ -1803,7 +1800,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>18</v>
@@ -1851,7 +1848,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>26</v>
@@ -1867,7 +1864,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>31</v>
@@ -1883,7 +1880,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>33</v>
@@ -1899,7 +1896,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>33</v>
@@ -1915,7 +1912,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
config and Test Case updated
</commit_message>
<xml_diff>
--- a/TestData/DriverHighLevelRegression.xlsx
+++ b/TestData/DriverHighLevelRegression.xlsx
@@ -1570,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1643,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
@@ -2091,7 +2091,7 @@
         <v>77</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>72</v>
@@ -2107,7 +2107,7 @@
         <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>72</v>
@@ -2123,7 +2123,7 @@
         <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>72</v>
@@ -2139,7 +2139,7 @@
         <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>72</v>
@@ -2187,7 +2187,7 @@
         <v>91</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>90</v>
@@ -2203,7 +2203,7 @@
         <v>94</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>90</v>
@@ -2219,7 +2219,7 @@
         <v>95</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>90</v>
@@ -2235,7 +2235,7 @@
         <v>93</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>88</v>
@@ -2251,7 +2251,7 @@
         <v>92</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>88</v>
@@ -2267,7 +2267,7 @@
         <v>103</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>97</v>
@@ -2283,7 +2283,7 @@
         <v>104</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>97</v>
@@ -2299,7 +2299,7 @@
         <v>105</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>100</v>
@@ -2315,7 +2315,7 @@
         <v>106</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>100</v>
@@ -2331,7 +2331,7 @@
         <v>107</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>100</v>
@@ -2347,7 +2347,7 @@
         <v>109</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>110</v>
@@ -2363,7 +2363,7 @@
         <v>112</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>110</v>
@@ -2379,7 +2379,7 @@
         <v>114</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>110</v>
@@ -2395,7 +2395,7 @@
         <v>130</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>110</v>
@@ -2411,7 +2411,7 @@
         <v>132</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>110</v>
@@ -2427,7 +2427,7 @@
         <v>200</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>110</v>
@@ -2443,7 +2443,7 @@
         <v>116</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>117</v>
@@ -2459,7 +2459,7 @@
         <v>119</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>117</v>
@@ -2475,7 +2475,7 @@
         <v>121</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>117</v>
@@ -2491,7 +2491,7 @@
         <v>123</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>124</v>
@@ -2507,7 +2507,7 @@
         <v>126</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>124</v>
@@ -2523,7 +2523,7 @@
         <v>128</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>124</v>
@@ -2539,7 +2539,7 @@
         <v>135</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>88</v>
@@ -2555,7 +2555,7 @@
         <v>137</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>88</v>
@@ -2571,7 +2571,7 @@
         <v>139</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>88</v>
@@ -2587,7 +2587,7 @@
         <v>144</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>145</v>
@@ -2603,7 +2603,7 @@
         <v>144</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>145</v>
@@ -2619,7 +2619,7 @@
         <v>144</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>145</v>
@@ -2635,7 +2635,7 @@
         <v>141</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>142</v>
@@ -2651,7 +2651,7 @@
         <v>149</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>142</v>
@@ -2667,7 +2667,7 @@
         <v>151</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>142</v>
@@ -2683,7 +2683,7 @@
         <v>153</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>154</v>
@@ -2699,7 +2699,7 @@
         <v>156</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>154</v>
@@ -2715,7 +2715,7 @@
         <v>158</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>159</v>
@@ -2731,7 +2731,7 @@
         <v>161</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>159</v>
@@ -2747,7 +2747,7 @@
         <v>163</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>159</v>
@@ -2763,7 +2763,7 @@
         <v>166</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>167</v>
@@ -2779,7 +2779,7 @@
         <v>166</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>167</v>
@@ -2795,7 +2795,7 @@
         <v>169</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>159</v>
@@ -2809,7 +2809,7 @@
         <v>171</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>159</v>
@@ -2823,7 +2823,7 @@
         <v>173</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>159</v>
@@ -2837,7 +2837,7 @@
         <v>175</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>176</v>
@@ -2851,7 +2851,7 @@
         <v>178</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>179</v>
@@ -2865,7 +2865,7 @@
         <v>181</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>182</v>
@@ -2879,7 +2879,7 @@
         <v>184</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>182</v>
@@ -2893,7 +2893,7 @@
         <v>186</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>182</v>
@@ -2907,7 +2907,7 @@
         <v>188</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>182</v>

</xml_diff>

<commit_message>
Config update for Edge  Browser
</commit_message>
<xml_diff>
--- a/TestData/DriverHighLevelRegression.xlsx
+++ b/TestData/DriverHighLevelRegression.xlsx
@@ -1570,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,7 +1611,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -1627,7 +1627,7 @@
         <v>207</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>206</v>
@@ -1643,7 +1643,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
@@ -1659,7 +1659,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>11</v>
@@ -1675,7 +1675,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
@@ -1691,7 +1691,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -1707,7 +1707,7 @@
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -1723,7 +1723,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -1739,7 +1739,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -1755,7 +1755,7 @@
         <v>192</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>190</v>
@@ -1771,7 +1771,7 @@
         <v>193</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>190</v>
@@ -1787,7 +1787,7 @@
         <v>197</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>198</v>
@@ -1803,7 +1803,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>18</v>
@@ -1819,7 +1819,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>22</v>
@@ -1835,7 +1835,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
@@ -1867,7 +1867,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>31</v>
@@ -1883,7 +1883,7 @@
         <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>33</v>
@@ -1899,7 +1899,7 @@
         <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>33</v>
@@ -1915,7 +1915,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>33</v>
@@ -1931,7 +1931,7 @@
         <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>58</v>
@@ -1947,7 +1947,7 @@
         <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>51</v>
@@ -1963,7 +1963,7 @@
         <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>54</v>
@@ -1979,7 +1979,7 @@
         <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>57</v>
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>195</v>
@@ -2011,7 +2011,7 @@
         <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>60</v>
@@ -2043,7 +2043,7 @@
         <v>202</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>203</v>
@@ -2059,7 +2059,7 @@
         <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>68</v>
@@ -2091,7 +2091,7 @@
         <v>77</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>72</v>
@@ -2107,7 +2107,7 @@
         <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>72</v>
@@ -2123,7 +2123,7 @@
         <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>72</v>
@@ -2139,7 +2139,7 @@
         <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>72</v>
@@ -2155,7 +2155,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>78</v>

</xml_diff>